<commit_message>
Updatd the Product Register script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-ProductRegister.data.xlsx
+++ b/tests/artifact/data/UI-ProductRegister.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="214">
   <si>
     <t>login.screen</t>
   </si>
@@ -460,7 +460,7 @@
     <t>From.Date</t>
   </si>
   <si>
-    <t>01-04-2023</t>
+    <t>15-11-2023</t>
   </si>
   <si>
     <t>ToDatefield.Name</t>
@@ -478,7 +478,7 @@
     <t>To.Date</t>
   </si>
   <si>
-    <t>31-03-2024</t>
+    <t>20-11-2023</t>
   </si>
   <si>
     <t>GodownField.Name</t>
@@ -625,13 +625,58 @@
     <t>//div[@class='mt-2']/div/table/tbody/tr[1]/td[2]/div/a/div</t>
   </si>
   <si>
-    <t>Invoice.number.heading</t>
+    <t>Invoice.name.heading</t>
   </si>
   <si>
     <t>//main[@class='mb-5']/section/div/div[2]/div/div/h5</t>
   </si>
   <si>
     <t>godown.Input.Values</t>
+  </si>
+  <si>
+    <t>Godown.enter.values</t>
+  </si>
+  <si>
+    <t>Primary Godown (Primary Godown's address)</t>
+  </si>
+  <si>
+    <t>godown.click.first.values</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div/div[2]/form/fieldset[2]/div/div/div/div/button[1]</t>
+  </si>
+  <si>
+    <t>filter.Table</t>
+  </si>
+  <si>
+    <t>//div[@class='popover-body']</t>
+  </si>
+  <si>
+    <t>filter.Table.heading</t>
+  </si>
+  <si>
+    <t>//div[@class='popover-body']/div[text()=' Invoice Type ']</t>
+  </si>
+  <si>
+    <t>Invoice.buyer.address</t>
+  </si>
+  <si>
+    <t>//main[@class='mb-5']/section/div/div[2]/div/div[2]/div/div/div/div[3]/div/div/p</t>
+  </si>
+  <si>
+    <t>searchValues</t>
+  </si>
+  <si>
+    <t>1/SL-23</t>
+  </si>
+  <si>
+    <t>search.invalid.values</t>
+  </si>
+  <si>
+    <t>filter.Popup.Message</t>
+  </si>
+  <si>
+    <t>//div[@class='toast-body'][contains(text(),'No data present for selected filter')]</t>
   </si>
 </sst>
 </file>
@@ -1746,10 +1791,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2587,6 +2632,67 @@
         <v>155</v>
       </c>
     </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>

<commit_message>
Updated Product Register Script
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-ProductRegister.data.xlsx
+++ b/tests/artifact/data/UI-ProductRegister.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -184,7 +184,7 @@
     <t>org.open</t>
   </si>
   <si>
-    <t>(//button[text()=' Open '])[107]</t>
+    <t>(//button[text()=' Open '])[108]</t>
   </si>
   <si>
     <t>org.hamburger</t>
@@ -1793,8 +1793,8 @@
   <sheetPr/>
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>

</xml_diff>

<commit_message>
Updated Product Register Script and raised few bugs
</commit_message>
<xml_diff>
--- a/tests/artifact/data/UI-ProductRegister.data.xlsx
+++ b/tests/artifact/data/UI-ProductRegister.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="216">
   <si>
     <t>login.screen</t>
   </si>
@@ -677,6 +677,12 @@
   </si>
   <si>
     <t>//div[@class='toast-body'][contains(text(),'No data present for selected filter')]</t>
+  </si>
+  <si>
+    <t>download.values</t>
+  </si>
+  <si>
+    <t>DownloadFile</t>
   </si>
 </sst>
 </file>
@@ -1791,10 +1797,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="125" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -2693,6 +2699,14 @@
         <v>213</v>
       </c>
     </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A25">

</xml_diff>